<commit_message>
Finally commiting for MOML
</commit_message>
<xml_diff>
--- a/dataset/hyper_paremetes.xlsx
+++ b/dataset/hyper_paremetes.xlsx
@@ -36,7 +36,7 @@
     <t xml:space="preserve">[ [32,16,8,4,],  [64,32,32,16,8, ],  [128,128,64,32,16,8,4, ],  [ 512,512,128,64,32,16,8,4, ] , ]</t>
   </si>
   <si>
-    <t xml:space="preserve">[ [2,4,8,16,32,64, ], [8,16,32,64,128,512,  ], [16,32, 64,128,512,1024, ], [32, 64,128,512,1024,2048,],  ]</t>
+    <t xml:space="preserve">[ [32,64,128,160,180,256, ], [64,80,128,256,270,364,  ], [80,100, 128,256,512,712, ], [128, 170,256,512,1024,2048,],  ]</t>
   </si>
   <si>
     <t>[7,5,5,3,3,3,]</t>
@@ -586,14 +586,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="19.28125"/>
-    <col customWidth="1" min="2" max="2" width="65.28125"/>
+    <col customWidth="1" min="2" max="2" width="84.7109375"/>
     <col customWidth="1" min="3" max="3" width="92.7109375"/>
     <col customWidth="1" min="4" max="4" width="23.8515625"/>
   </cols>

</xml_diff>